<commit_message>
Some big changes to the curriculum
</commit_message>
<xml_diff>
--- a/Plans/Plan for arbeid på Kuben V19.xlsx
+++ b/Plans/Plan for arbeid på Kuben V19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eirik\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eirik\Documents\KubenRobotics\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66F7BCE2-7616-44E7-8900-571C7CA823C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F5A26C-3E2A-475F-9C4C-A1D6DD313B9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="16070" xr2:uid="{CA229D0F-BE36-4CEC-83CC-16B2CDD4ABEE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="16065" xr2:uid="{CA229D0F-BE36-4CEC-83CC-16B2CDD4ABEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Hva</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Mal for prosjektrapport</t>
   </si>
   <si>
-    <t>Støttelitterstur I engelskfaget</t>
-  </si>
-  <si>
     <t>Matematiske dokumenter (quarternioner, komplekse tall etc)</t>
   </si>
   <si>
@@ -87,13 +84,28 @@
     <t>Jobbe med læreplan</t>
   </si>
   <si>
-    <t>Få på plass bestemt årsløpskombinasjon, koordinere/ha møte med Engelsklærer</t>
-  </si>
-  <si>
-    <t>Eirik: Lage støttelitteratur for engelskfaget, James: Kontorplass på Bitraf</t>
-  </si>
-  <si>
     <t>Planlegging av Halvåret &amp; Kontorplass på Bitraf</t>
+  </si>
+  <si>
+    <t>Eirik: Kontorplass på Bitraf + Lage støttelitteratur for engelskfaget, James: Kontorplass på Bitraf</t>
+  </si>
+  <si>
+    <t>Eirik: Kontorplass på Bitraf &amp; Møte med Sykkylven VGS, James: Møte med Sykkylven VGS + UR</t>
+  </si>
+  <si>
+    <t>Eirik: Kontorplass på Bitraf, James: Møter</t>
+  </si>
+  <si>
+    <t>Eirik: Kontorplass på Bitraf, James: Syk</t>
+  </si>
+  <si>
+    <t>Møte for å få på plass årsløpskombinasjon, samt møte med Engelsklærer om robotikk I engelsk</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Støttelitteratur I engelskfaget</t>
   </si>
 </sst>
 </file>
@@ -134,12 +146,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,11 +172,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -171,7 +186,16 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -491,19 +515,19 @@
   <dimension ref="B2:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="6" width="20.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="17" width="12.6328125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="8.7109375" style="1"/>
+    <col min="3" max="6" width="20.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1"/>
+    <col min="8" max="17" width="12.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -512,335 +536,343 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="I4" s="3" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="5">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
         <v>43483</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>43490</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="I5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="5">
-        <v>43490</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
       <c r="I6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="5">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
         <v>43497</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="5">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
         <v>43504</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="I8" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="5">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
         <v>43511</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
       <c r="I9" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
         <v>43518</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="I10" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
         <v>43525</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="I11" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
       <c r="M11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="5">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
         <v>43532</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="I12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="5">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
         <v>43539</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="I13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="5">
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
         <v>43546</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B15" s="5">
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
         <v>43553</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B16" s="5">
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
         <v>43560</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="5">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
         <v>43567</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="5">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="I17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
         <v>43574</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="5">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="I18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
         <v>43581</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="5">
+      <c r="C19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="I19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
         <v>43588</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="5">
+      <c r="C20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="I20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
         <v>43595</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="5">
+      <c r="C21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="I21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
         <v>43602</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="5">
+      <c r="C22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
         <v>43609</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="5">
+      <c r="C23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
         <v>43616</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="5">
+      <c r="C24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
         <v>43623</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="5">
+      <c r="C25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
         <v>43630</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="5">
+      <c r="C26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
         <v>43637</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="5">
+      <c r="C27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
         <v>43644</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
@@ -857,17 +889,6 @@
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="H7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>